<commit_message>
Se agrega condición para que que no grabe valores incorrectos en el log del balance
</commit_message>
<xml_diff>
--- a/BalanceDaily.xlsx
+++ b/BalanceDaily.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\MEmu Download\bot_ltc\ltcbot_telegram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B428D4DC-D3DD-401D-B167-63284A69356F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8403877E-838B-4A07-995D-CA8293925B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -120,8 +120,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{867B9B10-50FD-4FF7-B013-EBF27CDC5C3D}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{5132CE97-2AD6-40E0-932A-DE2AF17FE51F}" name="ValueLTC"/>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +504,66 @@
         <v>1.7469E-4</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44199</v>
+      </c>
+      <c r="B9">
+        <v>1.4957799999999999E-3</v>
+      </c>
+      <c r="C9" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B8,0),8)</f>
+        <v>1.5299000000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B10">
+        <v>1.62743E-3</v>
+      </c>
+      <c r="C10" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B9,0),8)</f>
+        <v>1.3165E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44201</v>
+      </c>
+      <c r="B11">
+        <v>1.7491E-3</v>
+      </c>
+      <c r="C11" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B10,0),8)</f>
+        <v>1.2167000000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44202</v>
+      </c>
+      <c r="B12">
+        <v>1.8720500000000001E-3</v>
+      </c>
+      <c r="C12" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B11,0),8)</f>
+        <v>1.2295000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44203</v>
+      </c>
+      <c r="B13">
+        <v>1.97919E-3</v>
+      </c>
+      <c r="C13" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B12,0),8)</f>
+        <v>1.0713999999999999E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregan nuevos bot y archivos de configuracion
</commit_message>
<xml_diff>
--- a/BalanceDaily.xlsx
+++ b/BalanceDaily.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\MEmu Download\bot_ltc\ltcbot_telegram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8403877E-838B-4A07-995D-CA8293925B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17045025-DD32-457B-9EEB-BDDE8B5E28FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -44,14 +45,18 @@
   <si>
     <t>IncrementDaily</t>
   </si>
+  <si>
+    <t>SpeedDailyByHour</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -90,16 +95,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
     </dxf>
@@ -120,13 +139,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:C13" totalsRowShown="0">
-  <autoFilter ref="A1:C13" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{867B9B10-50FD-4FF7-B013-EBF27CDC5C3D}" name="Date" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:D36" totalsRowShown="0">
+  <autoFilter ref="A1:D36" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{867B9B10-50FD-4FF7-B013-EBF27CDC5C3D}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{5132CE97-2AD6-40E0-932A-DE2AF17FE51F}" name="ValueLTC"/>
-    <tableColumn id="3" xr3:uid="{80AB9170-E305-4375-8C42-EDB0DB0AB414}" name="IncrementDaily" dataDxfId="0" dataCellStyle="Millares">
+    <tableColumn id="3" xr3:uid="{80AB9170-E305-4375-8C42-EDB0DB0AB414}" name="IncrementDaily" dataDxfId="4" dataCellStyle="Millares">
       <calculatedColumnFormula>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B1,0),8)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{911C793F-4670-443B-981F-AABED119AB31}" name="SpeedDailyByHour" dataDxfId="3">
+      <calculatedColumnFormula>BalanceDaily[[#This Row],[IncrementDaily]]/24</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C7AA665-B1E1-4D6B-8A11-E1AA6351B4C9}" name="BalanceDaily3" displayName="BalanceDaily3" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D3">
+    <sortCondition ref="A2:A3"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7C6F23C4-D84F-47C9-9707-97811061BF5E}" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1DD45AFC-C817-4D30-B50E-1414C10EE7EE}" name="ValueLTC"/>
+    <tableColumn id="3" xr3:uid="{AABFD8E3-2437-4368-831C-5BECE7B1E893}" name="IncrementDaily" dataDxfId="1" dataCellStyle="Millares">
+      <calculatedColumnFormula>ROUND(IFERROR(BalanceDaily3[[#This Row],[ValueLTC]]-B1,0),8)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{2D5492A8-C717-4A36-B691-D2D5B8D57AC4}" name="SpeedDailyByHour" dataDxfId="0">
+      <calculatedColumnFormula>BalanceDaily3[[#This Row],[IncrementDaily]]/24</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -396,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,9 +449,10 @@
     <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +462,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44192</v>
       </c>
@@ -431,8 +477,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B1,0),8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44193</v>
       </c>
@@ -443,8 +493,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B2,0),8)</f>
         <v>1.1828999999999999E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>4.92875E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44194</v>
       </c>
@@ -455,8 +509,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B3,0),8)</f>
         <v>7.2000000000000002E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>3.0000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44195</v>
       </c>
@@ -467,8 +525,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B4,0),8)</f>
         <v>1.4525000000000001E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>6.0520833333333333E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44196</v>
       </c>
@@ -479,8 +541,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B5,0),8)</f>
         <v>1.3202E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>5.5008333333333333E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44197</v>
       </c>
@@ -491,8 +557,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B6,0),8)</f>
         <v>2.61E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.0875E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44198</v>
       </c>
@@ -503,8 +573,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B7,0),8)</f>
         <v>1.7469E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>7.2787499999999996E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44199</v>
       </c>
@@ -515,8 +589,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B8,0),8)</f>
         <v>1.5299000000000001E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>6.3745833333333341E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44200</v>
       </c>
@@ -527,8 +605,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B9,0),8)</f>
         <v>1.3165E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>5.4854166666666667E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44201</v>
       </c>
@@ -539,8 +621,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B10,0),8)</f>
         <v>1.2167000000000001E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>5.0695833333333339E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44202</v>
       </c>
@@ -551,8 +637,12 @@
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B11,0),8)</f>
         <v>1.2295000000000001E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>5.1229166666666672E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44203</v>
       </c>
@@ -562,6 +652,449 @@
       <c r="C13" s="2">
         <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B12,0),8)</f>
         <v>1.0713999999999999E-4</v>
+      </c>
+      <c r="D13" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>4.4641666666666661E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44204</v>
+      </c>
+      <c r="B14">
+        <v>2.0857699999999998E-3</v>
+      </c>
+      <c r="C14" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B13,0),8)</f>
+        <v>1.0658E-4</v>
+      </c>
+      <c r="D14" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>4.4408333333333333E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44205</v>
+      </c>
+      <c r="B15">
+        <v>2.1864100000000002E-3</v>
+      </c>
+      <c r="C15" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B14,0),8)</f>
+        <v>1.0064E-4</v>
+      </c>
+      <c r="D15" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>4.1933333333333336E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44206</v>
+      </c>
+      <c r="B16">
+        <v>2.3489499999999998E-3</v>
+      </c>
+      <c r="C16" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B15,0),8)</f>
+        <v>1.6254E-4</v>
+      </c>
+      <c r="D16" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>6.7725E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44207</v>
+      </c>
+      <c r="B17">
+        <v>2.4980900000000001E-3</v>
+      </c>
+      <c r="C17" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B16,0),8)</f>
+        <v>1.4914E-4</v>
+      </c>
+      <c r="D17" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>6.2141666666666663E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44208</v>
+      </c>
+      <c r="B18">
+        <v>2.5953999999999999E-3</v>
+      </c>
+      <c r="C18" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B17,0),8)</f>
+        <v>9.7310000000000002E-5</v>
+      </c>
+      <c r="D18" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>4.0545833333333334E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44209</v>
+      </c>
+      <c r="B19">
+        <v>2.7463700000000001E-3</v>
+      </c>
+      <c r="C19" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B18,0),8)</f>
+        <v>1.5097E-4</v>
+      </c>
+      <c r="D19" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>6.2904166666666666E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44210</v>
+      </c>
+      <c r="B20">
+        <v>2.8869500000000001E-3</v>
+      </c>
+      <c r="C20" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B19,0),8)</f>
+        <v>1.4058000000000001E-4</v>
+      </c>
+      <c r="D20" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>5.8575000000000002E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44211</v>
+      </c>
+      <c r="B21">
+        <v>2.9676699999999999E-3</v>
+      </c>
+      <c r="C21" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B20,0),8)</f>
+        <v>8.072E-5</v>
+      </c>
+      <c r="D21" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>3.3633333333333335E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B22">
+        <v>3.1797000000000001E-3</v>
+      </c>
+      <c r="C22" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B21,0),8)</f>
+        <v>2.1202999999999999E-4</v>
+      </c>
+      <c r="D22" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>8.8345833333333334E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44213</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3.3114300000000002E-3</v>
+      </c>
+      <c r="C23" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B22,0),8)</f>
+        <v>1.3172999999999999E-4</v>
+      </c>
+      <c r="D23" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>5.4887499999999998E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B24">
+        <v>3.4714099999999999E-3</v>
+      </c>
+      <c r="C24" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B23,0),8)</f>
+        <v>1.5998E-4</v>
+      </c>
+      <c r="D24" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>6.6658333333333332E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44215</v>
+      </c>
+      <c r="B25">
+        <v>3.61474E-3</v>
+      </c>
+      <c r="C25" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B24,0),8)</f>
+        <v>1.4333E-4</v>
+      </c>
+      <c r="D25" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>5.9720833333333333E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44216</v>
+      </c>
+      <c r="B26">
+        <v>3.7877100000000001E-3</v>
+      </c>
+      <c r="C26" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B25,0),8)</f>
+        <v>1.7296999999999999E-4</v>
+      </c>
+      <c r="D26" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>7.2070833333333333E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44217</v>
+      </c>
+      <c r="B27">
+        <v>4.0840700000000004E-3</v>
+      </c>
+      <c r="C27" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B26,0),8)</f>
+        <v>2.9636000000000002E-4</v>
+      </c>
+      <c r="D27" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.2348333333333333E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44218</v>
+      </c>
+      <c r="B28">
+        <v>4.2607399999999998E-3</v>
+      </c>
+      <c r="C28" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B27,0),8)</f>
+        <v>1.7667E-4</v>
+      </c>
+      <c r="D28" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>7.36125E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>44219</v>
+      </c>
+      <c r="B29">
+        <v>4.4345799999999996E-3</v>
+      </c>
+      <c r="C29" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B28,0),8)</f>
+        <v>1.7384E-4</v>
+      </c>
+      <c r="D29" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>7.2433333333333332E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>44220</v>
+      </c>
+      <c r="B30">
+        <v>4.7063599999999997E-3</v>
+      </c>
+      <c r="C30" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B29,0),8)</f>
+        <v>2.7178E-4</v>
+      </c>
+      <c r="D30" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.1324166666666667E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>44221</v>
+      </c>
+      <c r="B31">
+        <v>4.8901099999999996E-3</v>
+      </c>
+      <c r="C31" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B30,0),8)</f>
+        <v>1.8374999999999999E-4</v>
+      </c>
+      <c r="D31" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>7.6562499999999998E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>44222</v>
+      </c>
+      <c r="B32">
+        <v>5.0876100000000002E-3</v>
+      </c>
+      <c r="C32" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B31,0),8)</f>
+        <v>1.975E-4</v>
+      </c>
+      <c r="D32" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>8.2291666666666674E-6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>44223</v>
+      </c>
+      <c r="B33">
+        <v>5.34806E-3</v>
+      </c>
+      <c r="C33" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B32,0),8)</f>
+        <v>2.6045000000000002E-4</v>
+      </c>
+      <c r="D33" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.0852083333333334E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>44224</v>
+      </c>
+      <c r="B34">
+        <v>5.5530800000000002E-3</v>
+      </c>
+      <c r="C34" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B33,0),8)</f>
+        <v>2.0502000000000001E-4</v>
+      </c>
+      <c r="D34" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>8.5424999999999999E-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>44225</v>
+      </c>
+      <c r="B35">
+        <v>5.8460200000000004E-3</v>
+      </c>
+      <c r="C35" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B34,0),8)</f>
+        <v>2.9294E-4</v>
+      </c>
+      <c r="D35" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.2205833333333333E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>44226</v>
+      </c>
+      <c r="B36">
+        <v>6.0276599999999998E-3</v>
+      </c>
+      <c r="C36" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B35,0),8)</f>
+        <v>1.8164E-4</v>
+      </c>
+      <c r="D36" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>7.5683333333333334E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCEDDE7-38BA-4BAF-9C6A-9E57D70428B0}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>44192</v>
+      </c>
+      <c r="B2">
+        <v>4.3953999999999998E-4</v>
+      </c>
+      <c r="C2" s="2">
+        <f>ROUND(IFERROR(BalanceDaily3[[#This Row],[ValueLTC]]-B1,0),8)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f>BalanceDaily3[[#This Row],[IncrementDaily]]/24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44223</v>
+      </c>
+      <c r="B3">
+        <v>5.34806E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <f>ROUND(IFERROR(BalanceDaily3[[#This Row],[ValueLTC]]-B2,0),8)</f>
+        <v>4.9085200000000004E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <f>BalanceDaily3[[#This Row],[IncrementDaily]]/24</f>
+        <v>2.0452166666666668E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan nuevos bot, el ultimo es el 129
</commit_message>
<xml_diff>
--- a/BalanceDaily.xlsx
+++ b/BalanceDaily.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\MEmu Download\bot_ltc\ltcbot_telegram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17045025-DD32-457B-9EEB-BDDE8B5E28FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58611D94-4D95-4CD7-98CA-174368BFAC42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -139,8 +139,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:D36" totalsRowShown="0">
-  <autoFilter ref="A1:D36" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:D42" totalsRowShown="0">
+  <autoFilter ref="A1:D42" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{867B9B10-50FD-4FF7-B013-EBF27CDC5C3D}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{5132CE97-2AD6-40E0-932A-DE2AF17FE51F}" name="ValueLTC"/>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,6 +1024,102 @@
       <c r="D36" s="3">
         <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
         <v>7.5683333333333334E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>44227</v>
+      </c>
+      <c r="B37">
+        <v>6.5768299999999997E-3</v>
+      </c>
+      <c r="C37" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B36,0),8)</f>
+        <v>5.4916999999999998E-4</v>
+      </c>
+      <c r="D37" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>2.2882083333333332E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B38">
+        <v>6.9079299999999996E-3</v>
+      </c>
+      <c r="C38" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B37,0),8)</f>
+        <v>3.3110000000000002E-4</v>
+      </c>
+      <c r="D38" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.3795833333333334E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>44229</v>
+      </c>
+      <c r="B39" s="4">
+        <v>7.2145600000000001E-3</v>
+      </c>
+      <c r="C39" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B38,0),8)</f>
+        <v>3.0663000000000001E-4</v>
+      </c>
+      <c r="D39" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.277625E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>44230</v>
+      </c>
+      <c r="B40">
+        <v>7.3893800000000001E-3</v>
+      </c>
+      <c r="C40" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B39,0),8)</f>
+        <v>1.7482000000000001E-4</v>
+      </c>
+      <c r="D40" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>7.2841666666666671E-6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B41">
+        <v>7.7778400000000003E-3</v>
+      </c>
+      <c r="C41" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B40,0),8)</f>
+        <v>3.8845999999999998E-4</v>
+      </c>
+      <c r="D41" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.6185833333333334E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>44232</v>
+      </c>
+      <c r="B42">
+        <v>8.0837900000000004E-3</v>
+      </c>
+      <c r="C42" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B41,0),8)</f>
+        <v>3.0594999999999998E-4</v>
+      </c>
+      <c r="D42" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>1.2747916666666665E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan nuevos bots
</commit_message>
<xml_diff>
--- a/BalanceDaily.xlsx
+++ b/BalanceDaily.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\MEmu Download\bot_ltc\ltcbot_telegram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58611D94-4D95-4CD7-98CA-174368BFAC42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D448E60A-4EC3-45EF-B98E-078420B7B214}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -139,8 +139,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:D42" totalsRowShown="0">
-  <autoFilter ref="A1:D42" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7C76C79-B42F-4CB0-9B2D-4E9113F1C61B}" name="BalanceDaily" displayName="BalanceDaily" ref="A1:D43" totalsRowShown="0">
+  <autoFilter ref="A1:D43" xr:uid="{91845030-72D7-4E0E-8F4D-35CD9A46DED9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{867B9B10-50FD-4FF7-B013-EBF27CDC5C3D}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{5132CE97-2AD6-40E0-932A-DE2AF17FE51F}" name="ValueLTC"/>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,6 +1120,22 @@
       <c r="D42" s="3">
         <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
         <v>1.2747916666666665E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>44233</v>
+      </c>
+      <c r="B43">
+        <v>8.6053699999999993E-3</v>
+      </c>
+      <c r="C43" s="2">
+        <f>ROUND(IFERROR(BalanceDaily[[#This Row],[ValueLTC]]-B42,0),8)</f>
+        <v>5.2158E-4</v>
+      </c>
+      <c r="D43" s="3">
+        <f>BalanceDaily[[#This Row],[IncrementDaily]]/24</f>
+        <v>2.1732499999999999E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>